<commit_message>
updated the Excel spreadsheet which calculates both liquid and various fixed-width layouts; removed the #VALUEs which show up in the tables at the unused slots.
</commit_message>
<xml_diff>
--- a/contrib/N-column-calculations-for-various-viewport-resolutions.xlsx
+++ b/contrib/N-column-calculations-for-various-viewport-resolutions.xlsx
@@ -15,8 +15,76 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Ger Hobbelt</author>
+  </authors>
+  <commentList>
+    <comment ref="C7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>width of the UI border when the browser window in spanning the platform viewport (width in pixels)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">width of vertical scrollbar alongside the page (in pixels)
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>the column number (1..n) for which to calculate the position</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C17" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">pick one of 1..4 to use that column width calculation
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>screen width:</t>
   </si>
@@ -53,24 +121,34 @@
   <si>
     <t>mult:</t>
   </si>
+  <si>
+    <t>column width, border + vscroll, rounddown:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
-    <numFmt numFmtId="166" formatCode="#.###%"/>
-    <numFmt numFmtId="168" formatCode="0.###"/>
-    <numFmt numFmtId="169" formatCode="0.###%"/>
-    <numFmt numFmtId="170" formatCode="0.0##%"/>
+    <numFmt numFmtId="164" formatCode="#.###%"/>
+    <numFmt numFmtId="165" formatCode="0.###"/>
+    <numFmt numFmtId="166" formatCode="0.###%"/>
+    <numFmt numFmtId="167" formatCode="0.0##%"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -111,20 +189,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,11 +506,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="AE20" sqref="AE20"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,7 +520,7 @@
     <col min="23" max="23" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
@@ -447,15 +528,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1">
-        <v>1920</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -463,19 +544,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>2</v>
       </c>
       <c r="C4">
-        <f>C2-C3</f>
-        <v>1920</v>
+        <f>MAX(0,C2-C3)</f>
+        <v>980</v>
       </c>
       <c r="D4" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -483,7 +564,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -491,7 +572,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>9</v>
       </c>
@@ -499,7 +580,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G9" t="s">
         <v>11</v>
       </c>
@@ -507,16 +588,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="11">
+        <v>1</v>
+      </c>
       <c r="B10" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="4">
-        <f>ROUNDDOWN(C4/C6,0)</f>
-        <v>80</v>
+        <f>IF(C6,ROUNDDOWN(C4/C6,0),0)</f>
+        <v>40</v>
       </c>
       <c r="D10" s="5">
-        <f>D4/C6</f>
+        <f>IF(C4,D4/C6,0)</f>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="E10" s="4"/>
@@ -524,62 +608,98 @@
       <c r="G10" s="4"/>
       <c r="H10" s="4">
         <f>$H$9*C10</f>
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="I10" s="5">
         <f>$H$9*D10</f>
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="11">
+        <v>2</v>
+      </c>
       <c r="B11" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="4">
-        <f>ROUNDDOWN((C4-C7)/C6,0)</f>
-        <v>79</v>
+        <f>IF(C6,ROUNDDOWN((C4-C7)/C6,0),0)</f>
+        <v>40</v>
       </c>
       <c r="D11" s="5">
-        <f>(D4-C7/C4)/C6</f>
-        <v>4.1623263888888887E-2</v>
+        <f>MAX(0,IF(AND(C4,C6),(D4-C7/C4)/C6,0))</f>
+        <v>4.1581632653061223E-2</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4">
         <f>$H$9*C10</f>
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="I11" s="5">
         <f>$H$9*D11</f>
-        <v>4.1623263888888887E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+        <v>4.1581632653061223E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="11">
+        <v>3</v>
+      </c>
       <c r="B12" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="4">
-        <f>ROUNDDOWN((C4-C8-C7)/C6,0)</f>
-        <v>79</v>
+        <f>IF(C6,MAX(0,ROUNDDOWN((C4-C8-C7)/C6,0)),0)</f>
+        <v>39</v>
       </c>
       <c r="D12" s="5">
-        <f>(D4-(C8+C7)/C4)/C6</f>
-        <v>4.118923611111111E-2</v>
+        <f>MAX(0,IF(AND(C4,C6),(D4-(C8+C7)/C4)/C6,0))</f>
+        <v>4.0731292517006801E-2</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4">
         <f>$H$9*C12</f>
-        <v>79</v>
+        <v>39</v>
       </c>
       <c r="I12" s="5">
         <f>$H$9*D12</f>
-        <v>4.118923611111111E-2</v>
+        <v>4.0731292517006801E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="11">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="4">
+        <f>ROUNDDOWN(C12/10,0)*10</f>
+        <v>30</v>
+      </c>
+      <c r="D13" s="5">
+        <f>IF(C4,C13/C4,0)</f>
+        <v>3.0612244897959183E-2</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4">
+        <f>ROUNDDOWN(H12/10,0)*10</f>
+        <v>30</v>
+      </c>
+      <c r="I13" s="5">
+        <f>$H$9*D13</f>
+        <v>3.0612244897959183E-2</v>
       </c>
     </row>
     <row r="17" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="C17" s="1">
+        <v>2</v>
+      </c>
       <c r="E17" t="s">
         <v>10</v>
       </c>
@@ -589,8 +709,8 @@
     </row>
     <row r="18" spans="1:38" x14ac:dyDescent="0.25">
       <c r="D18" s="10">
-        <f>I11</f>
-        <v>4.1623263888888887E-2</v>
+        <f>CHOOSE(C17,I10,I11,I12,I13)</f>
+        <v>4.1581632653061223E-2</v>
       </c>
       <c r="E18" s="8">
         <v>480</v>
@@ -638,8 +758,8 @@
         <v>1920</v>
       </c>
       <c r="W18" s="9">
-        <f>ROUNDDOWN(H11,0)</f>
-        <v>80</v>
+        <f>ROUNDDOWN(CHOOSE(C17,H10,H11,H12,H13),0)</f>
+        <v>40</v>
       </c>
       <c r="X18" s="8">
         <v>480</v>
@@ -806,7 +926,7 @@
         <v>span-2</v>
       </c>
       <c r="D20" s="8">
-        <f t="shared" ref="D20:D68" si="1">IF($A20&lt;=$C$6,$A20,"")</f>
+        <f t="shared" ref="D20:D42" si="1">IF($A20&lt;=$C$6,$A20,"")</f>
         <v>2</v>
       </c>
       <c r="E20" s="6">
@@ -855,7 +975,7 @@
         <v>8.3246527777777773E-2</v>
       </c>
       <c r="W20" s="8">
-        <f t="shared" ref="W20:W68" si="2">IF($A20&lt;=$C$6,$A20,"")</f>
+        <f t="shared" ref="W20:W42" si="2">IF($A20&lt;=$C$6,$A20,"")</f>
         <v>2</v>
       </c>
       <c r="X20" s="7">
@@ -6091,6 +6211,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>